<commit_message>
update to version 1.1 with detagging function
</commit_message>
<xml_diff>
--- a/Tag Excel List v.1.0.xlsx
+++ b/Tag Excel List v.1.0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>Person</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -349,6 +349,18 @@
   </si>
   <si>
     <t>Moffett, Samuel A.(마포삼열)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>렉 부인 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mrs. 렉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김 렉</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -704,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -1166,6 +1178,30 @@
       </c>
       <c r="B40" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>